<commit_message>
SUS Finale Score The End...
</commit_message>
<xml_diff>
--- a/Tasks/SUSStatistics.xlsx
+++ b/Tasks/SUSStatistics.xlsx
@@ -1,28 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\flights\Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3CFBA9B6-87DF-44FE-B8B3-21764AF06401}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD664F5-CE1E-49A4-9633-0AF2E71EBCCE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 απαντήσεις φόρμας" sheetId="1" r:id="rId1"/>
     <sheet name="1 3 5 7 9" sheetId="2" r:id="rId2"/>
     <sheet name="2 4 6 8 10" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Χρονική σήμανση</t>
   </si>
@@ -85,6 +92,9 @@
   </si>
   <si>
     <t>8) I found the website very cumbersome to use</t>
+  </si>
+  <si>
+    <t>SUS Score</t>
   </si>
 </sst>
 </file>
@@ -2989,11 +2999,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K25" activeCellId="5" sqref="A25:A28 C25:C28 E25:E28 G25:G28 I25:I28 K25:K28"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3561,7 +3571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>43469.789550844907</v>
       </c>
@@ -3596,7 +3606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>43470.325616840273</v>
       </c>
@@ -3631,7 +3641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>43470.394235763888</v>
       </c>
@@ -3666,7 +3676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>43471.660408738426</v>
       </c>
@@ -3701,7 +3711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>43471.660671284721</v>
       </c>
@@ -3736,7 +3746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>43471.669099155093</v>
       </c>
@@ -3771,7 +3781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>43472.47225820602</v>
       </c>
@@ -3806,7 +3816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -3840,8 +3850,11 @@
       <c r="K25" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="L25" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -3885,8 +3898,12 @@
         <f t="shared" si="0"/>
         <v>1.3636363636363635</v>
       </c>
+      <c r="L26" s="3">
+        <f>((B26-1)+(5-C26)+(D26-1)+(5-E26)+(F26-1)+(5-G26)+(H26-1)+(5-I26)+(J26-1)+(5-K26))*2.5</f>
+        <v>87.386363636363626</v>
+      </c>
     </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -3931,7 +3948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -4001,7 +4018,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0840D45-5BAB-4DC5-A58B-245D90F72DA9}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>

</xml_diff>